<commit_message>
feat(frontend): Finalize Bootstrap styles, fix table rendering, and set currency to LKR
</commit_message>
<xml_diff>
--- a/Samples/TestSheet01.xlsx
+++ b/Samples/TestSheet01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\ASP.NET\HRDataAPI_MAIN\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A977094D-DDA4-4F45-8403-9D2832DFF5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA74015-2877-481F-A77A-3188654D4334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EADC6B5C-DFBE-4AA2-9A52-E6E146B6478E}"/>
   </bookViews>
@@ -51,22 +51,22 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>Suran Sandeepa</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
     <t>70,000 LKR</t>
   </si>
   <si>
-    <t>Dilukshi</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
     <t>20,000 LKR</t>
+  </si>
+  <si>
+    <t>kamal</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>saman</t>
+  </si>
+  <si>
+    <t>flightops</t>
   </si>
 </sst>
 </file>
@@ -480,30 +480,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43479</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45729</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>46003</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>